<commit_message>
update info for ttest
</commit_message>
<xml_diff>
--- a/CD-valid/Input/Metadatatt.xlsx
+++ b/CD-valid/Input/Metadatatt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhabiby\Documents\GitHub\eu-data-validation\CD-valid\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA541C9F-28E2-42C0-BCE1-2426CA21D3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F80506E-3BCF-44F5-9803-3B4F443ABC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="196">
   <si>
     <t>variable</t>
   </si>
@@ -463,63 +463,6 @@
     <t>The news media. Please tell me, how much TRUST do you have in each of the following categories of people, groups of people, and institutions?</t>
   </si>
   <si>
-    <t>ATC_recruitment_public</t>
-  </si>
-  <si>
-    <t>2.4. Absence of nepotism, favoritism, and patronage</t>
-  </si>
-  <si>
-    <t>q2a</t>
-  </si>
-  <si>
-    <t>A public officer being recruited on the basis of family ties and friendship networks.</t>
-  </si>
-  <si>
-    <t>ATC_brbrequest_public</t>
-  </si>
-  <si>
-    <t>q2b</t>
-  </si>
-  <si>
-    <t>A public officer asking for a bribe to speed up administrative procedures.</t>
-  </si>
-  <si>
-    <t>ATC_brboffer_public</t>
-  </si>
-  <si>
-    <t>q2c</t>
-  </si>
-  <si>
-    <t>A private citizen offering a bribe to a public official to speed up administrative procedures.</t>
-  </si>
-  <si>
-    <t>ATC_embezz_priv</t>
-  </si>
-  <si>
-    <t>q2d</t>
-  </si>
-  <si>
-    <t>An elected official taking public funds for private use.</t>
-  </si>
-  <si>
-    <t>ATC_embezz_community</t>
-  </si>
-  <si>
-    <t>q2e</t>
-  </si>
-  <si>
-    <t>An elected official using stolen public funds to assist their community.</t>
-  </si>
-  <si>
-    <t>ATC_brbrequest_police</t>
-  </si>
-  <si>
-    <t>q2f</t>
-  </si>
-  <si>
-    <t>A law enforcement officer (police, customs, immigration, civil guard, military police) asking for a bribe.</t>
-  </si>
-  <si>
     <t>COR_prosecutors</t>
   </si>
   <si>
@@ -536,33 +479,6 @@
   </si>
   <si>
     <t>Public defense attorneys. How many of the following people in [COUNTRY] do you think are involved in corrupt practices?</t>
-  </si>
-  <si>
-    <t>COR_landreg</t>
-  </si>
-  <si>
-    <t>q3h</t>
-  </si>
-  <si>
-    <t>Land registry officers. How many of the following people in [COUNTRY] do you think are involved in corrupt practices?</t>
-  </si>
-  <si>
-    <t>COR_carreg</t>
-  </si>
-  <si>
-    <t>q3i</t>
-  </si>
-  <si>
-    <t>Car registration/driver license agency officers. How many of the following people in [COUNTRY] do you think are involved in corrupt practices?</t>
-  </si>
-  <si>
-    <t>COR_pparties</t>
-  </si>
-  <si>
-    <t>q3j</t>
-  </si>
-  <si>
-    <t>Political parties. How many of the following people in [COUNTRY] do you think are involved in corrupt practices?</t>
   </si>
   <si>
     <t>BRB_permit_A</t>
@@ -647,24 +563,6 @@
     <t>In practice, the government collaborates with civil society organizations in designing public policy. Do you agree or disagree that government collaboration with civil society is important for public policy design?</t>
   </si>
   <si>
-    <t>CPB_protest</t>
-  </si>
-  <si>
-    <t>q40_G2</t>
-  </si>
-  <si>
-    <t>Attended a legal demonstration or protest march?</t>
-  </si>
-  <si>
-    <t>CJP_effective</t>
-  </si>
-  <si>
-    <t>q44a_G1</t>
-  </si>
-  <si>
-    <t>Is effective in bringing people who commit crimes to justice. Please tell us how confident you are that the criminal justice system as a whole:</t>
-  </si>
-  <si>
     <t>CJP_efficient</t>
   </si>
   <si>
@@ -683,18 +581,6 @@
     <t>Makes sure everyone has access to the justice system if they need it. Please tell us how confident you are that the criminal justice system as a whole:</t>
   </si>
   <si>
-    <t>CJP_consistent</t>
-  </si>
-  <si>
-    <t>4.6. Justice</t>
-  </si>
-  <si>
-    <t>q44d_G1</t>
-  </si>
-  <si>
-    <t>Functions the same regardless of where you live? Please tell us how confident you are that the criminal justice system as a whole:</t>
-  </si>
-  <si>
     <t>CJP_fairpunishment</t>
   </si>
   <si>
@@ -707,9 +593,6 @@
     <t>CJP_egalitarian</t>
   </si>
   <si>
-    <t>8.5. Victim's Rights</t>
-  </si>
-  <si>
     <t>q44g_G1</t>
   </si>
   <si>
@@ -725,158 +608,13 @@
     <t>Provides victims of crime with the service and support they need. Please tell us how confident you are that the criminal justice system as a whole:</t>
   </si>
   <si>
-    <t>PAB_censorinfo</t>
-  </si>
-  <si>
-    <t>1.10. Respect for civil liberties (absence of authoritarianism)</t>
-  </si>
-  <si>
-    <t>q48_G1</t>
-  </si>
-  <si>
-    <t>censor information from abroad. Do you agree or disagree that censoring information from abroad is a concerning practice?</t>
-  </si>
-  <si>
-    <t>PAB_censorvoices</t>
-  </si>
-  <si>
-    <t>q49_G1</t>
-  </si>
-  <si>
-    <t>censor opposition voices domestically. Do you agree or disagree that censoring domestic opposition voices is a concerning practice?</t>
-  </si>
-  <si>
-    <t>PAB_blamesoc</t>
-  </si>
-  <si>
-    <t>q50_G1</t>
-  </si>
-  <si>
-    <t>blame different members or groups of society for domestic problems. Do you agree or disagree that blaming various societal groups for domestic issues is a concerning practice?</t>
-  </si>
-  <si>
-    <t>PAB_blameext</t>
-  </si>
-  <si>
-    <t>q51_G1</t>
-  </si>
-  <si>
-    <t>blame external forces (i.e., other countries, regional or 
-international governing bodies) for domestic problems. Do you agree or disagree that blaming external forces for domestic problems is a concerning practice?</t>
-  </si>
-  <si>
-    <t>PAB_freecourts</t>
-  </si>
-  <si>
-    <t>q52_G1</t>
-  </si>
-  <si>
-    <t>seek to limit the courts’ competences and freedom to interpret 
-the law. Do you agree or disagree that seeking to limit the courts' authority and interpretative freedom is a concerning practice?</t>
-  </si>
-  <si>
-    <t>PAB_judgeprom</t>
-  </si>
-  <si>
-    <t>q54_G1</t>
-  </si>
-  <si>
-    <t>seek to influence the promotion and removal of judges. Do you agree or disagree that seeking to influence the appointment and dismissal of judges is a concerning practice?</t>
-  </si>
-  <si>
-    <t>PAB_attackopp</t>
-  </si>
-  <si>
-    <t>q55_G1</t>
-  </si>
-  <si>
-    <t>attack or discredit opposition parties. Do you agree or disagree that attacking or discrediting opposition parties is a concerning practice?</t>
-  </si>
-  <si>
-    <t>PAB_prosecuteopp</t>
-  </si>
-  <si>
-    <t>q56_G1</t>
-  </si>
-  <si>
-    <t>prosecute and convict members of opposition parties. Do you agree or disagree that prosecuting and convicting members of opposition parties is a concerning practice?</t>
-  </si>
-  <si>
-    <t>LEP_polservpeopl</t>
-  </si>
-  <si>
-    <t>q43g_G2</t>
-  </si>
-  <si>
-    <t>The police in [COUNTRY] serve the interests of people like you. Do  you agree or disagree that the police serve the interests of individuals in your community, including people like you?</t>
-  </si>
-  <si>
-    <t>LEP_polservcom</t>
-  </si>
-  <si>
-    <t>q43h_G2</t>
-  </si>
-  <si>
-    <t>The police in [COUNTRY] serve the interests of your community. Do you agree or disagree that the police serve the interests of your local community?</t>
-  </si>
-  <si>
-    <t>PAB_distract</t>
-  </si>
-  <si>
-    <t>q49_G2</t>
-  </si>
-  <si>
-    <t>generate distractions from important issues and blame external enemies or internal traitors. Do you agree or disagree that distractions are created from critical matters while attributing domestic problems to external enemies or internal traitors?</t>
-  </si>
-  <si>
-    <t>PAB_credibility</t>
-  </si>
-  <si>
-    <t>q50_G2</t>
-  </si>
-  <si>
-    <t>deny criticisms and facts, and undermine the credibility of those presenting them.  Do you agree or disagree that criticisms and facts are denied and the credibility of those presenting them is undermined?</t>
-  </si>
-  <si>
-    <t>PAB_centralize</t>
-  </si>
-  <si>
-    <t>q51_G2</t>
-  </si>
-  <si>
-    <t>seek to centralize government functions and remove autonomy. Do you agree or disagree that efforts are made to centralize government functions and reduce autonomy of local authorities?
-from local authorities.</t>
-  </si>
-  <si>
-    <t>PAB_prosecutejourn</t>
-  </si>
-  <si>
-    <t>q53_G2</t>
-  </si>
-  <si>
-    <t>prosecute and convict journalists and leaders of civil society organizations that criticize them. Do you agree or disagree that journalists and leaders of civil society organizations who criticize certain entities are prosecuted and convicted?</t>
-  </si>
-  <si>
-    <t>PAB_attackelect</t>
-  </si>
-  <si>
-    <t>q55_G2</t>
-  </si>
-  <si>
-    <t>attack or discredit the electoral system and the electoral 
-supervisory organs. Do you agree or disagree that the electoral system and its supervisory organs are attacked or discredited?</t>
-  </si>
-  <si>
     <t>q57_G1 and q57_G2</t>
   </si>
   <si>
     <t>2.1: Absence of Bribery</t>
   </si>
   <si>
-    <t>1.06. Respect for the legitimacy of the constitutional order, the law making process, and political opponents (absence of authoritarianism)</t>
-  </si>
-  <si>
-    <t>1.09. Respect for the electoral process (absence of authoritarianism)</t>
+    <t>8.5: Victim's Rights</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1365,7 +1103,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>278</v>
+        <v>193</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -1376,7 +1114,7 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -1393,7 +1131,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -1410,7 +1148,7 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -1427,7 +1165,7 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -1444,7 +1182,7 @@
         <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
@@ -2141,186 +1879,186 @@
         <v>145</v>
       </c>
       <c r="B55" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="C55" t="s">
         <v>34</v>
       </c>
       <c r="D55" t="s">
+        <v>146</v>
+      </c>
+      <c r="E55" t="s">
         <v>147</v>
-      </c>
-      <c r="E55" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
-        <v>279</v>
+        <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="D56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E56" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C57" t="s">
         <v>34</v>
       </c>
       <c r="D57" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E57" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B58" t="s">
-        <v>279</v>
+        <v>121</v>
       </c>
       <c r="C58" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="D58" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E58" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C59" t="s">
         <v>34</v>
       </c>
       <c r="D59" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E59" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B60" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C60" t="s">
         <v>34</v>
       </c>
       <c r="D60" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E60" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="C61" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
       <c r="D61" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E61" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B62" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C62" t="s">
         <v>34</v>
       </c>
       <c r="D62" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E62" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>163</v>
+      </c>
+      <c r="B63" t="s">
+        <v>194</v>
+      </c>
+      <c r="C63" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" t="s">
         <v>164</v>
       </c>
-      <c r="B63" t="s">
-        <v>121</v>
-      </c>
-      <c r="C63" t="s">
-        <v>111</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>165</v>
-      </c>
-      <c r="E63" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B64" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C64" t="s">
         <v>34</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E64" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B65" t="s">
-        <v>121</v>
+        <v>194</v>
       </c>
       <c r="C65" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
       <c r="D65" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E65" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
@@ -2328,7 +2066,7 @@
         <v>170</v>
       </c>
       <c r="B66" t="s">
-        <v>279</v>
+        <v>194</v>
       </c>
       <c r="C66" t="s">
         <v>34</v>
@@ -2337,619 +2075,126 @@
         <v>171</v>
       </c>
       <c r="E66" t="s">
-        <v>172</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" t="s">
+        <v>75</v>
+      </c>
+      <c r="D67" t="s">
         <v>173</v>
       </c>
-      <c r="B67" t="s">
-        <v>279</v>
-      </c>
-      <c r="C67" t="s">
-        <v>34</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>174</v>
-      </c>
-      <c r="E67" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>175</v>
+      </c>
+      <c r="B68" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68" t="s">
         <v>176</v>
       </c>
-      <c r="B68" t="s">
-        <v>279</v>
-      </c>
-      <c r="C68" t="s">
-        <v>34</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>177</v>
-      </c>
-      <c r="E68" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>178</v>
+      </c>
+      <c r="B69" t="s">
+        <v>112</v>
+      </c>
+      <c r="C69" t="s">
+        <v>111</v>
+      </c>
+      <c r="D69" t="s">
         <v>179</v>
       </c>
-      <c r="B69" t="s">
-        <v>279</v>
-      </c>
-      <c r="C69" t="s">
-        <v>34</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>180</v>
-      </c>
-      <c r="E69" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>181</v>
+      </c>
+      <c r="B70" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" t="s">
+        <v>111</v>
+      </c>
+      <c r="D70" t="s">
         <v>182</v>
       </c>
-      <c r="B70" t="s">
-        <v>279</v>
-      </c>
-      <c r="C70" t="s">
-        <v>34</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>183</v>
-      </c>
-      <c r="E70" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>184</v>
+      </c>
+      <c r="B71" t="s">
+        <v>110</v>
+      </c>
+      <c r="C71" t="s">
+        <v>111</v>
+      </c>
+      <c r="D71" t="s">
         <v>185</v>
       </c>
-      <c r="B71" t="s">
-        <v>279</v>
-      </c>
-      <c r="C71" t="s">
-        <v>34</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>186</v>
-      </c>
-      <c r="E71" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>187</v>
+      </c>
+      <c r="B72" t="s">
+        <v>195</v>
+      </c>
+      <c r="C72" t="s">
+        <v>111</v>
+      </c>
+      <c r="D72" t="s">
         <v>188</v>
       </c>
-      <c r="B72" t="s">
-        <v>279</v>
-      </c>
-      <c r="C72" t="s">
-        <v>34</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>189</v>
-      </c>
-      <c r="E72" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>190</v>
+      </c>
+      <c r="B73" t="s">
+        <v>195</v>
+      </c>
+      <c r="C73" t="s">
+        <v>111</v>
+      </c>
+      <c r="D73" t="s">
         <v>191</v>
       </c>
-      <c r="B73" t="s">
-        <v>279</v>
-      </c>
-      <c r="C73" t="s">
-        <v>34</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>192</v>
-      </c>
-      <c r="E73" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>194</v>
-      </c>
-      <c r="B74" t="s">
-        <v>279</v>
-      </c>
-      <c r="C74" t="s">
-        <v>34</v>
-      </c>
-      <c r="D74" t="s">
-        <v>195</v>
-      </c>
-      <c r="E74" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>196</v>
-      </c>
-      <c r="B75" t="s">
-        <v>279</v>
-      </c>
-      <c r="C75" t="s">
-        <v>34</v>
-      </c>
-      <c r="D75" t="s">
-        <v>197</v>
-      </c>
-      <c r="E75" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>198</v>
-      </c>
-      <c r="B76" t="s">
-        <v>279</v>
-      </c>
-      <c r="C76" t="s">
-        <v>34</v>
-      </c>
-      <c r="D76" t="s">
-        <v>199</v>
-      </c>
-      <c r="E76" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>200</v>
-      </c>
-      <c r="B77" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" t="s">
-        <v>75</v>
-      </c>
-      <c r="D77" t="s">
-        <v>201</v>
-      </c>
-      <c r="E77" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>203</v>
-      </c>
-      <c r="B78" t="s">
-        <v>51</v>
-      </c>
-      <c r="C78" t="s">
-        <v>52</v>
-      </c>
-      <c r="D78" t="s">
-        <v>204</v>
-      </c>
-      <c r="E78" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>206</v>
-      </c>
-      <c r="B79" t="s">
-        <v>74</v>
-      </c>
-      <c r="C79" t="s">
-        <v>75</v>
-      </c>
-      <c r="D79" t="s">
-        <v>207</v>
-      </c>
-      <c r="E79" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>209</v>
-      </c>
-      <c r="B80" t="s">
-        <v>112</v>
-      </c>
-      <c r="C80" t="s">
-        <v>111</v>
-      </c>
-      <c r="D80" t="s">
-        <v>210</v>
-      </c>
-      <c r="E80" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>212</v>
-      </c>
-      <c r="B81" t="s">
-        <v>112</v>
-      </c>
-      <c r="C81" t="s">
-        <v>111</v>
-      </c>
-      <c r="D81" t="s">
-        <v>213</v>
-      </c>
-      <c r="E81" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>215</v>
-      </c>
-      <c r="B82" t="s">
-        <v>112</v>
-      </c>
-      <c r="C82" t="s">
-        <v>111</v>
-      </c>
-      <c r="D82" t="s">
-        <v>216</v>
-      </c>
-      <c r="E82" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>218</v>
-      </c>
-      <c r="B83" t="s">
-        <v>219</v>
-      </c>
-      <c r="C83" t="s">
-        <v>75</v>
-      </c>
-      <c r="D83" t="s">
-        <v>220</v>
-      </c>
-      <c r="E83" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>218</v>
-      </c>
-      <c r="B84" t="s">
-        <v>112</v>
-      </c>
-      <c r="C84" t="s">
-        <v>111</v>
-      </c>
-      <c r="D84" t="s">
-        <v>220</v>
-      </c>
-      <c r="E84" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>222</v>
-      </c>
-      <c r="B85" t="s">
-        <v>110</v>
-      </c>
-      <c r="C85" t="s">
-        <v>111</v>
-      </c>
-      <c r="D85" t="s">
-        <v>223</v>
-      </c>
-      <c r="E85" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>225</v>
-      </c>
-      <c r="B86" t="s">
-        <v>226</v>
-      </c>
-      <c r="C86" t="s">
-        <v>111</v>
-      </c>
-      <c r="D86" t="s">
-        <v>227</v>
-      </c>
-      <c r="E86" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>229</v>
-      </c>
-      <c r="B87" t="s">
-        <v>226</v>
-      </c>
-      <c r="C87" t="s">
-        <v>111</v>
-      </c>
-      <c r="D87" t="s">
-        <v>230</v>
-      </c>
-      <c r="E87" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>232</v>
-      </c>
-      <c r="B88" t="s">
-        <v>233</v>
-      </c>
-      <c r="C88" t="s">
-        <v>7</v>
-      </c>
-      <c r="D88" t="s">
-        <v>234</v>
-      </c>
-      <c r="E88" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>236</v>
-      </c>
-      <c r="B89" t="s">
-        <v>233</v>
-      </c>
-      <c r="C89" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" t="s">
-        <v>237</v>
-      </c>
-      <c r="E89" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>239</v>
-      </c>
-      <c r="B90" t="s">
-        <v>233</v>
-      </c>
-      <c r="C90" t="s">
-        <v>7</v>
-      </c>
-      <c r="D90" t="s">
-        <v>240</v>
-      </c>
-      <c r="E90" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>242</v>
-      </c>
-      <c r="B91" t="s">
-        <v>233</v>
-      </c>
-      <c r="C91" t="s">
-        <v>7</v>
-      </c>
-      <c r="D91" t="s">
-        <v>243</v>
-      </c>
-      <c r="E91" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>245</v>
-      </c>
-      <c r="B92" t="s">
-        <v>233</v>
-      </c>
-      <c r="C92" t="s">
-        <v>7</v>
-      </c>
-      <c r="D92" t="s">
-        <v>246</v>
-      </c>
-      <c r="E92" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>248</v>
-      </c>
-      <c r="B93" t="s">
-        <v>281</v>
-      </c>
-      <c r="C93" t="s">
-        <v>7</v>
-      </c>
-      <c r="D93" t="s">
-        <v>249</v>
-      </c>
-      <c r="E93" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>251</v>
-      </c>
-      <c r="B94" t="s">
-        <v>281</v>
-      </c>
-      <c r="C94" t="s">
-        <v>7</v>
-      </c>
-      <c r="D94" t="s">
-        <v>252</v>
-      </c>
-      <c r="E94" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>254</v>
-      </c>
-      <c r="B95" t="s">
-        <v>233</v>
-      </c>
-      <c r="C95" t="s">
-        <v>7</v>
-      </c>
-      <c r="D95" t="s">
-        <v>255</v>
-      </c>
-      <c r="E95" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>257</v>
-      </c>
-      <c r="B96" t="s">
-        <v>101</v>
-      </c>
-      <c r="C96" t="s">
-        <v>102</v>
-      </c>
-      <c r="D96" t="s">
-        <v>258</v>
-      </c>
-      <c r="E96" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>260</v>
-      </c>
-      <c r="B97" t="s">
-        <v>101</v>
-      </c>
-      <c r="C97" t="s">
-        <v>102</v>
-      </c>
-      <c r="D97" t="s">
-        <v>261</v>
-      </c>
-      <c r="E97" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>263</v>
-      </c>
-      <c r="B98" t="s">
-        <v>233</v>
-      </c>
-      <c r="C98" t="s">
-        <v>7</v>
-      </c>
-      <c r="D98" t="s">
-        <v>264</v>
-      </c>
-      <c r="E98" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>266</v>
-      </c>
-      <c r="B99" t="s">
-        <v>233</v>
-      </c>
-      <c r="C99" t="s">
-        <v>7</v>
-      </c>
-      <c r="D99" t="s">
-        <v>267</v>
-      </c>
-      <c r="E99" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>269</v>
-      </c>
-      <c r="B100" t="s">
-        <v>280</v>
-      </c>
-      <c r="C100" t="s">
-        <v>7</v>
-      </c>
-      <c r="D100" t="s">
-        <v>270</v>
-      </c>
-      <c r="E100" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>272</v>
-      </c>
-      <c r="B101" t="s">
-        <v>233</v>
-      </c>
-      <c r="C101" t="s">
-        <v>7</v>
-      </c>
-      <c r="D101" t="s">
-        <v>273</v>
-      </c>
-      <c r="E101" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>275</v>
-      </c>
-      <c r="B102" t="s">
-        <v>281</v>
-      </c>
-      <c r="C102" t="s">
-        <v>7</v>
-      </c>
-      <c r="D102" t="s">
-        <v>276</v>
-      </c>
-      <c r="E102" t="s">
-        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>